<commit_message>
added scaling nutrient uptake analysis
</commit_message>
<xml_diff>
--- a/stats/NEC_NCPModels.xlsx
+++ b/stats/NEC_NCPModels.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nyssa\Desktop\CRANE-R\stats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsilbiger\Desktop\CRANE-R\stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12890" windowHeight="8040" tabRatio="742"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12885" windowHeight="8040" tabRatio="742" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="81">
   <si>
     <t>Net</t>
   </si>
@@ -213,18 +213,12 @@
     <t>NCP:Nutrient LevelHigh:SubstrateSand</t>
   </si>
   <si>
-    <t>Summary</t>
-  </si>
-  <si>
     <t>Sum Sq</t>
   </si>
   <si>
     <t>Mean Sq</t>
   </si>
   <si>
-    <t>ANOVA</t>
-  </si>
-  <si>
     <t>Aragonite Staturation</t>
   </si>
   <si>
@@ -237,15 +231,9 @@
     <t>Aragonite Staturation:Nutrient LevelHigh</t>
   </si>
   <si>
-    <t xml:space="preserve">Table S1: Summary results from mixed effects model for net ecosystem calcification models from net (24 hours), daytime, and nighttime samples. </t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
-    <t xml:space="preserve">Table S2: Summary results from mixed effects model for net community production models from net (24 hours), daytime (gross community production = NCP - R), and nighttime (respiration) samples. </t>
-  </si>
-  <si>
     <t>(a) ANOVA Table</t>
   </si>
   <si>
@@ -258,21 +246,21 @@
     <t>(b) Summary</t>
   </si>
   <si>
-    <t xml:space="preserve">Table S4:  Algae: (a) ANOVA table and (b) summary results for NEC as a function of nutrient level by aragonite saturation state. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Table S5:  Coral: (a) ANOVA table and (b) summary results for NEC as a function of nutrient level by aragonite saturation state. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Table S6:  Rubble: (a) ANOVA table and (b) summary results for NEC as a function of nutrient level by aragonite saturation state. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Table S7:  Sand: (a) ANOVA table and (b) summary results for NEC as a function of nutrient level by aragonite saturation state. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Table S8: Mixed:  (a) ANOVA table and (b) summary results for NEC as a function of nutrient level by aragonite saturation state. </t>
-  </si>
-  <si>
+    <t>&lt;0.0001</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Table S1: Summary results from mixed effects model for net community calcification models from net (24 hours), daytime, and nighttime samples. Bold p-values are significant at the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">α </t>
+    </r>
     <r>
       <rPr>
         <sz val="12"/>
@@ -280,7 +268,18 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Table S3: (a) ANOVA table and (b) summary results for pH as a function of NCP x substrate x nutrient level.</t>
+      <t>&lt; 0.05 level.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Table S3: (a) ANOVA table and (b) summary results for pH as a function of NCP by substrate by nutrient level.</t>
     </r>
     <r>
       <rPr>
@@ -289,11 +288,29 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve">  Bold p-values are significant at the α &lt; 0.05 level.</t>
     </r>
   </si>
   <si>
-    <t>&lt;0.0001</t>
+    <t>Table S4:  Algae: (a) ANOVA table and (b) summary results for NCC as a function of nutrient level by aragonite saturation state.  Bold p-values are significant at the α &lt; 0.05 level.</t>
+  </si>
+  <si>
+    <t>Table S5:  Coral: (a) ANOVA table and (b) summary results for NCC as a function of nutrient level by aragonite saturation state.  Bold p-values are significant at the α &lt; 0.05 level.</t>
+  </si>
+  <si>
+    <t>Table S6:  Rubble: (a) ANOVA table and (b) summary results for NCC as a function of nutrient level by aragonite saturation state.  Bold p-values are significant at the α &lt; 0.05 level.</t>
+  </si>
+  <si>
+    <t>Table S7:  Sand: (a) ANOVA table and (b) summary results for NCC as a function of nutrient level by aragonite saturation state.  Bold p-values are significant at the α &lt; 0.05 level.</t>
+  </si>
+  <si>
+    <t>Table S8: Mixed:  (a) ANOVA table and (b) summary results for NCC as a function of nutrient level by aragonite saturation state.  Bold p-values are significant at the α &lt; 0.05 level.</t>
+  </si>
+  <si>
+    <t>&gt;0.001</t>
+  </si>
+  <si>
+    <t>Table S2: Summary results from mixed effects model for net community production models from net (24 hours), daytime (gross community production = NCP - R), and nighttime (respiration) samples.  Bold p-values are significant at the α &lt; 0.05 level.</t>
   </si>
 </sst>
 </file>
@@ -303,7 +320,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,6 +359,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -978,15 +1001,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="73" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B1" s="74"/>
       <c r="C1" s="74"/>
@@ -996,7 +1019,7 @@
       <c r="G1" s="74"/>
       <c r="H1" s="74"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -1020,7 +1043,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1032,127 +1055,127 @@
       <c r="G3" s="7"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="11">
-        <v>461.17703995357903</v>
+        <v>431.956480148575</v>
       </c>
       <c r="D4" s="11">
-        <v>230.58851997679</v>
+        <v>215.97824007428699</v>
       </c>
       <c r="E4" s="10">
         <v>2</v>
       </c>
       <c r="F4" s="12">
-        <v>51.999991274348197</v>
+        <v>52</v>
       </c>
       <c r="G4" s="11">
-        <v>32.2367471478372</v>
+        <v>29.734548480490201</v>
       </c>
       <c r="H4" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="11">
-        <v>65.632337828497</v>
+        <v>66.896017343386404</v>
       </c>
       <c r="D5" s="11">
-        <v>32.8161689142485</v>
+        <v>33.448008671693202</v>
       </c>
       <c r="E5" s="10">
         <v>2</v>
       </c>
       <c r="F5" s="12">
-        <v>54.000001683219402</v>
+        <v>54.000000298071797</v>
       </c>
       <c r="G5" s="11">
-        <v>21.9208046172138</v>
+        <v>22.861633053059101</v>
       </c>
       <c r="H5" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="11">
-        <v>7.4725755220809704</v>
+        <v>6.2592550910610303</v>
       </c>
       <c r="D6" s="11">
-        <v>3.7362877610404799</v>
+        <v>3.1296275455305098</v>
       </c>
       <c r="E6" s="10">
         <v>2</v>
       </c>
       <c r="F6" s="12">
-        <v>54.000002495635897</v>
+        <v>54.000002647486802</v>
       </c>
       <c r="G6" s="11">
-        <v>5.5312530134182296</v>
+        <v>4.6938258080179702</v>
       </c>
       <c r="H6" s="23">
         <v>6.5267992521513803E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="11">
-        <v>57.470371887360997</v>
+        <v>54.152223783063903</v>
       </c>
       <c r="D7" s="11">
-        <v>28.735185943680499</v>
+        <v>27.076111891531902</v>
       </c>
       <c r="E7" s="10">
         <v>2</v>
       </c>
       <c r="F7" s="12">
-        <v>53.999984313870897</v>
+        <v>53.9999968421129</v>
       </c>
       <c r="G7" s="11">
-        <v>6.9209423764169902</v>
+        <v>6.1986681748422399</v>
       </c>
       <c r="H7" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="11">
-        <v>255.70138275105899</v>
+        <v>262.29405046811598</v>
       </c>
       <c r="D8" s="11">
-        <v>127.85069137553</v>
+        <v>131.14702523405799</v>
       </c>
       <c r="E8" s="10">
         <v>2</v>
       </c>
       <c r="F8" s="12">
-        <v>240.999983488151</v>
+        <v>241.000026341812</v>
       </c>
       <c r="G8" s="11">
-        <v>75.713473516730303</v>
+        <v>75.0763475124227</v>
       </c>
       <c r="H8" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -1164,127 +1187,127 @@
       <c r="G9" s="15"/>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="11">
-        <v>327.08068205331301</v>
+        <v>302.57608366191801</v>
       </c>
       <c r="D10" s="11">
-        <v>163.54034102665699</v>
+        <v>151.288041830959</v>
       </c>
       <c r="E10" s="10">
         <v>2</v>
       </c>
       <c r="F10" s="12">
-        <v>27.9999933119066</v>
+        <v>28</v>
       </c>
       <c r="G10" s="11">
-        <v>18.897472228196499</v>
+        <v>16.903859889676301</v>
       </c>
       <c r="H10" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="11">
-        <v>59.873482010583402</v>
+        <v>54.471428701736798</v>
       </c>
       <c r="D11" s="11">
-        <v>29.936741005291701</v>
+        <v>27.235714350868399</v>
       </c>
       <c r="E11" s="10">
         <v>2</v>
       </c>
       <c r="F11" s="12">
-        <v>30.000001283142701</v>
+        <v>30.000000522365202</v>
       </c>
       <c r="G11" s="11">
-        <v>34.588193874712601</v>
+        <v>29.965409637868198</v>
       </c>
       <c r="H11" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="11">
-        <v>6.5373296764944104</v>
+        <v>5.4178944541464196</v>
       </c>
       <c r="D12" s="11">
-        <v>3.2686648382471999</v>
+        <v>2.7089472270732098</v>
       </c>
       <c r="E12" s="10">
         <v>2</v>
       </c>
       <c r="F12" s="12">
-        <v>30.000000272742199</v>
+        <v>30.000000523622901</v>
       </c>
       <c r="G12" s="11">
-        <v>4.8874812750856904</v>
+        <v>4.0682523781961599</v>
       </c>
       <c r="H12" s="23">
-        <v>1.4543606900023799E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="11">
-        <v>41.819464742717003</v>
+        <v>37.114820399741802</v>
       </c>
       <c r="D13" s="11">
-        <v>20.909732371358501</v>
+        <v>18.557410199870901</v>
       </c>
       <c r="E13" s="10">
         <v>2</v>
       </c>
       <c r="F13" s="12">
-        <v>28.000000915372599</v>
+        <v>28.0000007875827</v>
       </c>
       <c r="G13" s="11">
-        <v>3.7790284984559301</v>
+        <v>3.2833416401987301</v>
       </c>
       <c r="H13" s="23">
-        <v>3.5243589094357798E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="11">
-        <v>132.46559863951401</v>
+        <v>129.55081891384799</v>
       </c>
       <c r="D14" s="11">
-        <v>66.232799319757206</v>
+        <v>64.775409456924095</v>
       </c>
       <c r="E14" s="10">
         <v>2</v>
       </c>
       <c r="F14" s="12">
-        <v>135.999996289916</v>
+        <v>136.000009482731</v>
       </c>
       <c r="G14" s="11">
-        <v>35.437496333220103</v>
+        <v>34.056524495441899</v>
       </c>
       <c r="H14" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>14</v>
       </c>
@@ -1296,121 +1319,121 @@
       <c r="G15" s="15"/>
       <c r="H15" s="24"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="11">
-        <v>142.49485419999999</v>
+        <v>136.844724514467</v>
       </c>
       <c r="D16" s="11">
-        <v>71.247427110000004</v>
+        <v>68.422362257233303</v>
       </c>
       <c r="E16" s="10">
         <v>2</v>
       </c>
       <c r="F16" s="12">
-        <v>19.999997919999998</v>
+        <v>19.999999125143901</v>
       </c>
       <c r="G16" s="11">
-        <v>13.819695299999999</v>
+        <v>13.5701973227366</v>
       </c>
       <c r="H16" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="11">
-        <v>17.266084930000002</v>
+        <v>21.727998090115101</v>
       </c>
       <c r="D17" s="11">
-        <v>8.6330424650000008</v>
+        <v>10.8639990450576</v>
       </c>
       <c r="E17" s="10">
         <v>2</v>
       </c>
       <c r="F17" s="12">
-        <v>21.999999110000001</v>
+        <v>22.000001251296901</v>
       </c>
       <c r="G17" s="11">
-        <v>4.3795282740000001</v>
-      </c>
-      <c r="H17" s="23">
-        <v>2.5057999000000001E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <v>5.6323529073990199</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="11">
-        <v>1.7225706199999999</v>
+        <v>1.62965208945439</v>
       </c>
       <c r="D18" s="11">
-        <v>0.86128530999999997</v>
+        <v>0.814826044727196</v>
       </c>
       <c r="E18" s="10">
         <v>2</v>
       </c>
       <c r="F18" s="12">
-        <v>22.00000103</v>
+        <v>21.999999768441398</v>
       </c>
       <c r="G18" s="11">
-        <v>1.2126537479999999</v>
+        <v>1.1762440440264901</v>
       </c>
       <c r="H18" s="13">
-        <v>0.31652575199999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="11">
-        <v>23.631557269999998</v>
+        <v>27.7574771704795</v>
       </c>
       <c r="D19" s="11">
-        <v>11.815778630000001</v>
+        <v>13.8787385852397</v>
       </c>
       <c r="E19" s="10">
         <v>2</v>
       </c>
       <c r="F19" s="12">
-        <v>19.99999948</v>
+        <v>19.999998650585699</v>
       </c>
       <c r="G19" s="11">
-        <v>6.1525392840000004</v>
+        <v>6.3459307459172596</v>
       </c>
       <c r="H19" s="23">
         <v>8.2716460000000006E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="20">
-        <v>124.0488536</v>
+        <v>134.50156049689099</v>
       </c>
       <c r="D20" s="20">
-        <v>62.024426800000001</v>
+        <v>67.250780248445693</v>
       </c>
       <c r="E20" s="19">
         <v>2</v>
       </c>
       <c r="F20" s="21">
-        <v>102.9999981</v>
+        <v>102.99999802487299</v>
       </c>
       <c r="G20" s="20">
-        <v>43.798215429999999</v>
+        <v>44.885201250972202</v>
       </c>
       <c r="H20" s="25" t="s">
         <v>16</v>
@@ -1430,14 +1453,14 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="73" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B1" s="74"/>
       <c r="C1" s="74"/>
@@ -1447,7 +1470,7 @@
       <c r="G1" s="74"/>
       <c r="H1" s="74"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -1471,7 +1494,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1483,130 +1506,129 @@
       <c r="G3" s="32"/>
       <c r="H3" s="33"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="29" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="30">
-        <v>22.730516269999999</v>
+        <v>31.527486723865898</v>
       </c>
       <c r="D4" s="30">
-        <v>11.365258130000001</v>
+        <v>15.763743361932899</v>
       </c>
       <c r="E4" s="29">
         <v>2</v>
       </c>
       <c r="F4" s="31">
-        <v>54.000773870000003</v>
+        <v>53.9996883396417</v>
       </c>
       <c r="G4" s="30">
-        <v>8.9819125E-2</v>
+        <v>0.124462206627644</v>
       </c>
       <c r="H4" s="34">
-        <v>0.91423277800000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.88322418884189102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="11">
-        <v>9.5948015360000003</v>
+        <v>10.3912073248087</v>
       </c>
       <c r="D5" s="11">
-        <v>4.7974007680000001</v>
+        <v>5.1956036624043698</v>
       </c>
       <c r="E5" s="10">
         <v>2</v>
       </c>
       <c r="F5" s="12">
-        <v>51.999843660000003</v>
+        <v>52.000297938942502</v>
       </c>
       <c r="G5" s="11">
-        <v>4.3846291000000003E-2</v>
+        <v>4.7611969686194598E-2</v>
       </c>
       <c r="H5" s="13">
-        <v>0.95713640700000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.95354522088872495</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="11">
-        <v>23.46676167</v>
+        <v>25.9330542781411</v>
       </c>
       <c r="D6" s="11">
-        <v>11.73338083</v>
+        <v>12.9665271390706</v>
       </c>
       <c r="E6" s="10">
         <v>2</v>
       </c>
       <c r="F6" s="12">
-        <v>52.000051749999997</v>
+        <v>51.999962921296799</v>
       </c>
       <c r="G6" s="11">
-        <v>1.02615583</v>
+        <v>1.1382150202988199</v>
       </c>
       <c r="H6" s="13">
-        <v>0.36552395900000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.32824173327772999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="11">
-        <v>86.974528699999993</v>
+        <v>80.390677518764207</v>
       </c>
       <c r="D7" s="11">
-        <v>43.487264349999997</v>
+        <v>40.195338759382103</v>
       </c>
       <c r="E7" s="10">
         <v>2</v>
       </c>
       <c r="F7" s="12">
-        <v>51.99996256</v>
+        <v>51.999994163164601</v>
       </c>
       <c r="G7" s="11">
-        <v>0.81882043000000004</v>
+        <v>0.75881842406733802</v>
       </c>
       <c r="H7" s="13">
-        <v>0.44655562999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
-        <v>15</v>
-      </c>
+        <v>0.47333301802926703</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="11">
-        <v>89.840103119999995</v>
+        <v>87.985650984714496</v>
       </c>
       <c r="D8" s="11">
-        <v>44.920051559999997</v>
+        <v>43.992825492357198</v>
       </c>
       <c r="E8" s="10">
         <v>2</v>
       </c>
       <c r="F8" s="12">
-        <v>240.99976150000001</v>
+        <v>240.99970953150401</v>
       </c>
       <c r="G8" s="11">
-        <v>0.98060528599999996</v>
+        <v>0.95967774392058902</v>
       </c>
       <c r="H8" s="13">
-        <v>0.37657546600000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
+        <v>0.384475039309497</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -1615,130 +1637,129 @@
       <c r="G9" s="15"/>
       <c r="H9" s="17"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="29" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="30">
-        <v>1229.5639269999999</v>
+        <v>1228.12067705249</v>
       </c>
       <c r="D10" s="30">
-        <v>614.78196330000003</v>
+        <v>614.060338526245</v>
       </c>
       <c r="E10" s="29">
         <v>2</v>
       </c>
       <c r="F10" s="31">
-        <v>28.00014981</v>
+        <v>27.999671648649599</v>
       </c>
       <c r="G10" s="30">
-        <v>3.2656391149999999</v>
+        <v>3.2550032604249499</v>
       </c>
       <c r="H10" s="36">
         <v>5.3117129999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="11">
-        <v>869.13873430000001</v>
+        <v>830.86425780545596</v>
       </c>
       <c r="D11" s="11">
-        <v>434.56936719999999</v>
+        <v>415.43212890272798</v>
       </c>
       <c r="E11" s="10">
         <v>2</v>
       </c>
       <c r="F11" s="12">
-        <v>27.99991468</v>
+        <v>27.999607579542801</v>
       </c>
       <c r="G11" s="11">
-        <v>2.9897089939999999</v>
+        <v>2.8595272054118701</v>
       </c>
       <c r="H11" s="13">
         <v>6.6556375000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="11">
-        <v>35.235848439999998</v>
+        <v>32.357311359387097</v>
       </c>
       <c r="D12" s="11">
-        <v>17.617924219999999</v>
+        <v>16.178655679693598</v>
       </c>
       <c r="E12" s="10">
         <v>2</v>
       </c>
       <c r="F12" s="12">
-        <v>28.000038279999998</v>
+        <v>28.000021673109401</v>
       </c>
       <c r="G12" s="11">
-        <v>0.98704167700000001</v>
+        <v>0.90863003352650396</v>
       </c>
       <c r="H12" s="13">
-        <v>0.38527397200000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="11">
-        <v>2111.0881159999999</v>
+        <v>2141.3979358511701</v>
       </c>
       <c r="D13" s="11">
-        <v>1055.5440579999999</v>
+        <v>1070.6989679255901</v>
       </c>
       <c r="E13" s="10">
         <v>2</v>
       </c>
       <c r="F13" s="12">
-        <v>28.00002126</v>
+        <v>27.999916053808299</v>
       </c>
       <c r="G13" s="11">
-        <v>18.551872670000002</v>
+        <v>18.4803642761124</v>
       </c>
       <c r="H13" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="9" t="s">
-        <v>69</v>
-      </c>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="11">
-        <v>1737.5725090000001</v>
+        <v>1638.88264484448</v>
       </c>
       <c r="D14" s="11">
-        <v>868.7862543</v>
+        <v>819.44132242223804</v>
       </c>
       <c r="E14" s="10">
         <v>2</v>
       </c>
       <c r="F14" s="12">
-        <v>136.00025400000001</v>
+        <v>135.999952600461</v>
       </c>
       <c r="G14" s="11">
-        <v>13.52112245</v>
+        <v>12.7565399181363</v>
       </c>
       <c r="H14" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="6"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1747,124 +1768,124 @@
       <c r="G15" s="15"/>
       <c r="H15" s="17"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="29" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="30">
-        <v>311.4421734</v>
+        <v>317.94897867494302</v>
       </c>
       <c r="D16" s="30">
-        <v>155.7210867</v>
+        <v>158.974489337471</v>
       </c>
       <c r="E16" s="29">
         <v>2</v>
       </c>
       <c r="F16" s="31">
-        <v>20.000001709999999</v>
+        <v>20.000011450229898</v>
       </c>
       <c r="G16" s="30">
-        <v>9.9523844409999995</v>
+        <v>9.9977104765933902</v>
       </c>
       <c r="H16" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="11">
-        <v>152.9805503</v>
+        <v>141.584954598331</v>
       </c>
       <c r="D17" s="11">
-        <v>76.490275150000002</v>
+        <v>70.792477299165597</v>
       </c>
       <c r="E17" s="10">
         <v>2</v>
       </c>
       <c r="F17" s="12">
-        <v>19.999995819999999</v>
+        <v>19.999995240172701</v>
       </c>
       <c r="G17" s="11">
-        <v>9.6125663170000006</v>
+        <v>9.0400010840296705</v>
       </c>
       <c r="H17" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="11">
-        <v>30.415887300000001</v>
+        <v>30.366048625955099</v>
       </c>
       <c r="D18" s="11">
-        <v>15.207943650000001</v>
+        <v>15.183024312977601</v>
       </c>
       <c r="E18" s="10">
         <v>2</v>
       </c>
       <c r="F18" s="12">
-        <v>21.99999961</v>
+        <v>21.999999685427799</v>
       </c>
       <c r="G18" s="11">
-        <v>6.8288046040000001</v>
+        <v>6.7592668868579597</v>
       </c>
       <c r="H18" s="23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="11">
-        <v>404.54365780000001</v>
+        <v>389.62720839938999</v>
       </c>
       <c r="D19" s="11">
-        <v>202.2718289</v>
+        <v>194.81360419969499</v>
       </c>
       <c r="E19" s="10">
         <v>2</v>
       </c>
       <c r="F19" s="12">
-        <v>21.99999949</v>
+        <v>20.0000085300717</v>
       </c>
       <c r="G19" s="11">
-        <v>33.625979579999999</v>
+        <v>34.468733562383498</v>
       </c>
       <c r="H19" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
       <c r="B20" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="20">
-        <v>18.829347599999998</v>
+        <v>17.299073830872899</v>
       </c>
       <c r="D20" s="20">
-        <v>9.4146737980000008</v>
+        <v>8.6495369154364301</v>
       </c>
       <c r="E20" s="19">
         <v>2</v>
       </c>
       <c r="F20" s="21">
-        <v>103.0000756</v>
+        <v>103.000105186675</v>
       </c>
       <c r="G20" s="20">
-        <v>0.63653806400000001</v>
+        <v>0.58749546959450205</v>
       </c>
       <c r="H20" s="22">
-        <v>0.53118953099999999</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -1880,19 +1901,19 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.81640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="40.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="75" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B1" s="76"/>
       <c r="C1" s="76"/>
@@ -1901,9 +1922,9 @@
       <c r="F1" s="76"/>
       <c r="G1" s="76"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B2" s="40"/>
       <c r="C2" s="40"/>
@@ -1912,7 +1933,7 @@
       <c r="F2" s="40"/>
       <c r="G2" s="41"/>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A3" s="42"/>
       <c r="B3" s="26" t="s">
         <v>28</v>
@@ -1933,7 +1954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
         <v>30</v>
       </c>
@@ -1956,7 +1977,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>31</v>
       </c>
@@ -1979,7 +2000,7 @@
         <v>1.537E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
         <v>1</v>
       </c>
@@ -2002,7 +2023,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
         <v>32</v>
       </c>
@@ -2025,7 +2046,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
         <v>33</v>
       </c>
@@ -2048,7 +2069,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="43" t="s">
         <v>34</v>
       </c>
@@ -2071,7 +2092,7 @@
         <v>0.68661000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="45" t="s">
         <v>35</v>
       </c>
@@ -2094,12 +2115,12 @@
         <v>0.65895999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="38"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="47" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B12" s="40"/>
       <c r="C12" s="40"/>
@@ -2107,7 +2128,7 @@
       <c r="E12" s="40"/>
       <c r="F12" s="41"/>
     </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A13" s="42"/>
       <c r="B13" s="26" t="s">
         <v>18</v>
@@ -2125,7 +2146,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="42" t="s">
         <v>20</v>
       </c>
@@ -2145,7 +2166,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
         <v>30</v>
       </c>
@@ -2165,7 +2186,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="42" t="s">
         <v>40</v>
       </c>
@@ -2185,7 +2206,7 @@
         <v>0.35177126413438198</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="42" t="s">
         <v>41</v>
       </c>
@@ -2205,7 +2226,7 @@
         <v>0.29199837761178399</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="42" t="s">
         <v>21</v>
       </c>
@@ -2225,7 +2246,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
         <v>22</v>
       </c>
@@ -2245,7 +2266,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="42" t="s">
         <v>23</v>
       </c>
@@ -2265,7 +2286,7 @@
         <v>0.29176264490803999</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="42" t="s">
         <v>24</v>
       </c>
@@ -2285,7 +2306,7 @@
         <v>0.32529352274283801</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="42" t="s">
         <v>42</v>
       </c>
@@ -2305,7 +2326,7 @@
         <v>0.13022742340221999</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
         <v>43</v>
       </c>
@@ -2325,7 +2346,7 @@
         <v>7.3566875917844901E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="42" t="s">
         <v>36</v>
       </c>
@@ -2345,7 +2366,7 @@
         <v>5.6107620431839998E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="42" t="s">
         <v>37</v>
       </c>
@@ -2365,7 +2386,7 @@
         <v>9.3674854597343399E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="42" t="s">
         <v>38</v>
       </c>
@@ -2385,7 +2406,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="42" t="s">
         <v>39</v>
       </c>
@@ -2405,7 +2426,7 @@
         <v>0.143783285038866</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="42" t="s">
         <v>44</v>
       </c>
@@ -2425,7 +2446,7 @@
         <v>0.45876993268340299</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="42" t="s">
         <v>45</v>
       </c>
@@ -2445,7 +2466,7 @@
         <v>0.50766878788699099</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="s">
         <v>46</v>
       </c>
@@ -2465,7 +2486,7 @@
         <v>0.45603499471203901</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
         <v>47</v>
       </c>
@@ -2485,7 +2506,7 @@
         <v>0.46194230353636201</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="42" t="s">
         <v>48</v>
       </c>
@@ -2505,7 +2526,7 @@
         <v>0.62546835131473399</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="42" t="s">
         <v>49</v>
       </c>
@@ -2525,7 +2546,7 @@
         <v>0.82417285124645001</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="42" t="s">
         <v>50</v>
       </c>
@@ -2545,7 +2566,7 @@
         <v>0.90149277428850305</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="42" t="s">
         <v>51</v>
       </c>
@@ -2565,7 +2586,7 @@
         <v>0.95469572922366897</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>52</v>
       </c>
@@ -2585,7 +2606,7 @@
         <v>0.93907816381427101</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="42" t="s">
         <v>53</v>
       </c>
@@ -2605,7 +2626,7 @@
         <v>0.53262989203264699</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="42" t="s">
         <v>54</v>
       </c>
@@ -2625,7 +2646,7 @@
         <v>0.32280303333206301</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="42" t="s">
         <v>55</v>
       </c>
@@ -2645,7 +2666,7 @@
         <v>0.62439769599270201</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="42" t="s">
         <v>56</v>
       </c>
@@ -2665,7 +2686,7 @@
         <v>0.302791771514413</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="42" t="s">
         <v>57</v>
       </c>
@@ -2685,7 +2706,7 @@
         <v>0.29701866148440598</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="42" t="s">
         <v>58</v>
       </c>
@@ -2705,7 +2726,7 @@
         <v>0.14368846045410499</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="48" t="s">
         <v>59</v>
       </c>
@@ -2739,18 +2760,18 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.1796875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="38.140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="75" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="76"/>
       <c r="C1" s="76"/>
@@ -2759,9 +2780,9 @@
       <c r="F1" s="76"/>
       <c r="G1" s="76"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
@@ -2770,13 +2791,13 @@
       <c r="F2" s="50"/>
       <c r="G2" s="51"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="52"/>
       <c r="B3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>62</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>4</v>
@@ -2791,15 +2812,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" s="11">
-        <v>1.6899999999999998E-2</v>
+        <v>0.46</v>
       </c>
       <c r="C4" s="11">
-        <v>1.6899999999999998E-2</v>
+        <v>0.46</v>
       </c>
       <c r="D4" s="10">
         <v>1</v>
@@ -2808,21 +2829,21 @@
         <v>57</v>
       </c>
       <c r="F4" s="11">
-        <v>7.1000000000000004E-3</v>
+        <v>0.19</v>
       </c>
       <c r="G4" s="71">
-        <v>0.93298000000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="11">
-        <v>6.9198000000000004</v>
+        <v>6.71</v>
       </c>
       <c r="C5" s="11">
-        <v>3.4599000000000002</v>
+        <v>3.36</v>
       </c>
       <c r="D5" s="10">
         <v>2</v>
@@ -2831,21 +2852,21 @@
         <v>57</v>
       </c>
       <c r="F5" s="11">
-        <v>1.4589000000000001</v>
+        <v>1.37</v>
       </c>
       <c r="G5" s="71">
-        <v>0.24104999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" s="11">
-        <v>16.466999999999999</v>
+        <v>14.15</v>
       </c>
       <c r="C6" s="11">
-        <v>8.2334999999999994</v>
+        <v>7.07</v>
       </c>
       <c r="D6" s="10">
         <v>2</v>
@@ -2854,13 +2875,13 @@
         <v>57</v>
       </c>
       <c r="F6" s="11">
-        <v>3.4716</v>
-      </c>
-      <c r="G6" s="72">
-        <v>3.7780000000000001E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>2.89</v>
+      </c>
+      <c r="G6" s="71">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="54"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -2869,9 +2890,9 @@
       <c r="F7" s="10"/>
       <c r="G7" s="53"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="55" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -2880,7 +2901,7 @@
       <c r="F8" s="14"/>
       <c r="G8" s="56"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="54"/>
       <c r="B9" s="10" t="s">
         <v>18</v>
@@ -2899,142 +2920,142 @@
       </c>
       <c r="G9" s="53"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="54" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="11">
-        <v>0.74303549822628701</v>
+        <v>0.86745950170645303</v>
       </c>
       <c r="C10" s="11">
-        <v>1.4054399004214799</v>
+        <v>1.42781269163252</v>
       </c>
       <c r="D10" s="10">
-        <v>56.9999973087887</v>
+        <v>56.999998981490897</v>
       </c>
       <c r="E10" s="11">
-        <v>0.52868535894238899</v>
+        <v>0.60754432762088995</v>
       </c>
       <c r="F10" s="62">
-        <v>0.599076421387578</v>
+        <v>0.54590265830559903</v>
       </c>
       <c r="G10" s="53"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" s="11">
-        <v>4.9204353513708103E-2</v>
+        <v>6.8640358047333594E-2</v>
       </c>
       <c r="C11" s="11">
-        <v>0.44391029808387</v>
+        <v>0.45097677770528999</v>
       </c>
       <c r="D11" s="10">
-        <v>56.999997308778397</v>
+        <v>56.999998981538702</v>
       </c>
       <c r="E11" s="11">
-        <v>0.11084300978395401</v>
+        <v>0.15220375292181801</v>
       </c>
       <c r="F11" s="62">
-        <v>0.91213021247636294</v>
+        <v>0.87956370722052302</v>
       </c>
       <c r="G11" s="53"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="54" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="11">
-        <v>-2.6279660597768002</v>
+        <v>-2.7987110433731499</v>
       </c>
       <c r="C12" s="11">
-        <v>1.8009842923049799</v>
+        <v>1.82965364026786</v>
       </c>
       <c r="D12" s="10">
-        <v>56.999997308741598</v>
+        <v>56.999998981511403</v>
       </c>
       <c r="E12" s="11">
-        <v>-1.45918322053404</v>
+        <v>-1.5296398082007601</v>
       </c>
       <c r="F12" s="62">
-        <v>0.15000389715651499</v>
+        <v>0.131637071510468</v>
       </c>
       <c r="G12" s="53"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="54" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="11">
-        <v>-0.37621118437770501</v>
+        <v>-0.81475972518034601</v>
       </c>
       <c r="C13" s="11">
-        <v>1.76165455268532</v>
+        <v>1.78969782190045</v>
       </c>
       <c r="D13" s="10">
-        <v>56.999997308829997</v>
+        <v>56.999998981478498</v>
       </c>
       <c r="E13" s="11">
-        <v>-0.21355559397512899</v>
+        <v>-0.45524988364525398</v>
       </c>
       <c r="F13" s="62">
-        <v>0.83165566718511297</v>
+        <v>0.65065888040433295</v>
       </c>
       <c r="G13" s="53"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="54" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B14" s="11">
-        <v>0.57047265641702705</v>
+        <v>0.61275955748603805</v>
       </c>
       <c r="C14" s="11">
-        <v>0.56090479558283701</v>
+        <v>0.569833676765932</v>
       </c>
       <c r="D14" s="10">
-        <v>56.999997308712999</v>
+        <v>56.999998981535697</v>
       </c>
       <c r="E14" s="11">
-        <v>1.01705790520876</v>
+        <v>1.07533054375398</v>
       </c>
       <c r="F14" s="62">
-        <v>0.313423570619906</v>
+        <v>0.28675753363134199</v>
       </c>
       <c r="G14" s="53"/>
     </row>
-    <row r="15" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="57" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B15" s="20">
-        <v>-0.66351869185685497</v>
+        <v>-0.53365790664026502</v>
       </c>
       <c r="C15" s="20">
-        <v>0.54752740022894897</v>
+        <v>0.55624333052520103</v>
       </c>
       <c r="D15" s="19">
-        <v>56.999997308750501</v>
+        <v>56.999998981483699</v>
       </c>
       <c r="E15" s="20">
-        <v>-1.2118456383724401</v>
+        <v>-0.95939650393001397</v>
       </c>
       <c r="F15" s="63">
-        <v>0.230571174140661</v>
+        <v>0.34141106227115298</v>
       </c>
       <c r="G15" s="58"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="37"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="37"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="37"/>
     </row>
   </sheetData>
@@ -3051,17 +3072,17 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.54296875" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="73" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B1" s="74"/>
       <c r="C1" s="74"/>
@@ -3070,9 +3091,9 @@
       <c r="F1" s="74"/>
       <c r="G1" s="74"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
@@ -3082,13 +3103,13 @@
       <c r="G2" s="51"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="52"/>
       <c r="B3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>62</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>4</v>
@@ -3104,79 +3125,79 @@
       </c>
       <c r="H3" s="37"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" s="11">
-        <v>564.57000000000005</v>
+        <v>606.07000000000005</v>
       </c>
       <c r="C4" s="11">
-        <v>564.57000000000005</v>
+        <v>606.07000000000005</v>
       </c>
       <c r="D4" s="10">
         <v>1</v>
       </c>
       <c r="E4" s="11">
-        <v>51.066000000000003</v>
+        <v>51.16</v>
       </c>
       <c r="F4" s="11">
-        <v>81.040000000000006</v>
+        <v>86.85</v>
       </c>
       <c r="G4" s="72" t="s">
         <v>16</v>
       </c>
       <c r="H4" s="37"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="11">
-        <v>5.3</v>
+        <v>6.74</v>
       </c>
       <c r="C5" s="11">
-        <v>2.65</v>
+        <v>3.37</v>
       </c>
       <c r="D5" s="10">
         <v>2</v>
       </c>
       <c r="E5" s="11">
-        <v>47.398000000000003</v>
+        <v>46.73</v>
       </c>
       <c r="F5" s="11">
-        <v>0.38</v>
+        <v>0.48</v>
       </c>
       <c r="G5" s="71">
         <v>0.68572</v>
       </c>
       <c r="H5" s="37"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" s="11">
-        <v>66.260000000000005</v>
+        <v>69.760000000000005</v>
       </c>
       <c r="C6" s="11">
-        <v>33.130000000000003</v>
+        <v>34.880000000000003</v>
       </c>
       <c r="D6" s="10">
         <v>2</v>
       </c>
       <c r="E6" s="11">
-        <v>51.042999999999999</v>
+        <v>51.402000000000001</v>
       </c>
       <c r="F6" s="11">
-        <v>4.7549999999999999</v>
+        <v>5</v>
       </c>
       <c r="G6" s="72">
-        <v>1.277E-2</v>
+        <v>0.01</v>
       </c>
       <c r="H6" s="37"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="54"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -3186,9 +3207,9 @@
       <c r="G7" s="53"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="55" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
@@ -3198,7 +3219,7 @@
       <c r="G8" s="56"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="54"/>
       <c r="B9" s="29" t="s">
         <v>18</v>
@@ -3218,134 +3239,134 @@
       <c r="G9" s="53"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="54" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="11">
-        <v>-4.4967439992107003</v>
+        <v>-4.5595121593784604</v>
       </c>
       <c r="C10" s="11">
-        <v>2.9466913530038901</v>
+        <v>2.9576704664952298</v>
       </c>
       <c r="D10" s="11">
-        <v>41.390359485880403</v>
+        <v>40.961172136136597</v>
       </c>
       <c r="E10" s="11">
-        <v>-1.52603155896415</v>
+        <v>-1.5415889670702201</v>
       </c>
       <c r="F10" s="62">
-        <v>0.13460794152302299</v>
+        <v>0.13086444518389301</v>
       </c>
       <c r="G10" s="53"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" s="11">
-        <v>6.2278202817085102</v>
+        <v>6.3838929300212204</v>
       </c>
       <c r="C11" s="11">
-        <v>0.99335838553803002</v>
+        <v>0.99419534932502196</v>
       </c>
       <c r="D11" s="11">
-        <v>51.045043886845598</v>
+        <v>51.043461605611299</v>
       </c>
       <c r="E11" s="11">
-        <v>6.2694596153586097</v>
+        <v>6.4211655529824903</v>
       </c>
       <c r="F11" s="69" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="G11" s="53"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="54" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="11">
-        <v>3.5927982638377903E-2</v>
+        <v>7.6851469405916001E-2</v>
       </c>
       <c r="C12" s="11">
-        <v>3.8323513435752701</v>
+        <v>3.8457713020484898</v>
       </c>
       <c r="D12" s="11">
-        <v>51.137049110157903</v>
+        <v>50.670533242895701</v>
       </c>
       <c r="E12" s="11">
-        <v>9.3749187945956994E-3</v>
+        <v>1.99833696208041E-2</v>
       </c>
       <c r="F12" s="62">
-        <v>0.99255648554110698</v>
+        <v>0.98413512295664696</v>
       </c>
       <c r="G12" s="53"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="54" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="11">
-        <v>2.4679218647368502</v>
+        <v>2.81321522053346</v>
       </c>
       <c r="C13" s="11">
-        <v>3.4617110071903001</v>
+        <v>3.47591410597671</v>
       </c>
       <c r="D13" s="11">
-        <v>47.387877524211099</v>
+        <v>46.709393465348398</v>
       </c>
       <c r="E13" s="11">
-        <v>0.71291966880272195</v>
+        <v>0.80934543684385996</v>
       </c>
       <c r="F13" s="62">
-        <v>0.47939152793152501</v>
+        <v>0.422420253451049</v>
       </c>
       <c r="G13" s="53"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="54" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B14" s="11">
-        <v>-1.5319905855893701</v>
+        <v>-1.44973501741989</v>
       </c>
       <c r="C14" s="11">
-        <v>1.3569000767517601</v>
+        <v>1.3580409406977001</v>
       </c>
       <c r="D14" s="11">
-        <v>51.038669398290097</v>
+        <v>51.037445911964099</v>
       </c>
       <c r="E14" s="11">
-        <v>-1.1290371427030601</v>
+        <v>-1.0675193758702699</v>
       </c>
       <c r="F14" s="62">
-        <v>0.264161013713679</v>
+        <v>0.29076097429021103</v>
       </c>
       <c r="G14" s="53"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="57" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B15" s="20">
-        <v>-3.5458587668136698</v>
+        <v>-3.6050100295723899</v>
       </c>
       <c r="C15" s="20">
-        <v>1.19598136729521</v>
+        <v>1.1969896131982101</v>
       </c>
       <c r="D15" s="20">
-        <v>51.0462547643397</v>
+        <v>51.044577993544301</v>
       </c>
       <c r="E15" s="20">
-        <v>-2.9648110445339699</v>
+        <v>-3.0117304192308199</v>
       </c>
       <c r="F15" s="70">
-        <v>4.5950469645021901E-3</v>
+        <v>4.0334922995768404E-3</v>
       </c>
       <c r="G15" s="58"/>
     </row>
@@ -3362,17 +3383,17 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.453125" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="73" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="74"/>
       <c r="C1" s="74"/>
@@ -3381,9 +3402,9 @@
       <c r="F1" s="74"/>
       <c r="G1" s="74"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
@@ -3392,13 +3413,13 @@
       <c r="F2" s="50"/>
       <c r="G2" s="51"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="52"/>
       <c r="B3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>62</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>4</v>
@@ -3413,76 +3434,76 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" s="11">
-        <v>55.02</v>
+        <v>58.75</v>
       </c>
       <c r="C4" s="11">
-        <v>55.02</v>
+        <v>58.75</v>
       </c>
       <c r="D4" s="10">
         <v>1</v>
       </c>
       <c r="E4" s="11">
-        <v>51.863</v>
+        <v>51.82</v>
       </c>
       <c r="F4" s="11">
-        <v>71.094999999999999</v>
+        <v>76.95</v>
       </c>
       <c r="G4" s="27" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="11">
-        <v>2.2050000000000001</v>
+        <v>1.19</v>
       </c>
       <c r="C5" s="11">
-        <v>1.103</v>
+        <v>0.97</v>
       </c>
       <c r="D5" s="10">
         <v>2</v>
       </c>
       <c r="E5" s="11">
-        <v>56.755000000000003</v>
+        <v>56.7</v>
       </c>
       <c r="F5" s="11">
-        <v>1.425</v>
+        <v>1.27</v>
       </c>
       <c r="G5" s="71">
-        <v>0.249</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" s="11">
-        <v>3.4260000000000002</v>
+        <v>2.94</v>
       </c>
       <c r="C6" s="11">
-        <v>1.7130000000000001</v>
+        <v>1.47</v>
       </c>
       <c r="D6" s="10">
         <v>2</v>
       </c>
       <c r="E6" s="11">
-        <v>52.024999999999999</v>
+        <v>51.98</v>
       </c>
       <c r="F6" s="11">
-        <v>2.2130000000000001</v>
+        <v>1.94</v>
       </c>
       <c r="G6" s="71">
-        <v>0.1195</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="54"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -3491,9 +3512,9 @@
       <c r="F7" s="10"/>
       <c r="G7" s="53"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="55" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -3502,7 +3523,7 @@
       <c r="F8" s="14"/>
       <c r="G8" s="56"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="54"/>
       <c r="B9" s="10" t="s">
         <v>18</v>
@@ -3521,129 +3542,129 @@
       </c>
       <c r="G9" s="53"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="54" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="11">
-        <v>-7.6588945055454296</v>
+        <v>-7.5733605066359901</v>
       </c>
       <c r="C10" s="11">
-        <v>1.3570052686332399</v>
+        <v>1.3500729185095901</v>
       </c>
       <c r="D10" s="11">
-        <v>56.123586549996098</v>
+        <v>56.248953690796299</v>
       </c>
       <c r="E10" s="11">
-        <v>-5.6439681426288102</v>
+        <v>-5.6095936766116203</v>
       </c>
       <c r="F10" s="69" t="s">
         <v>16</v>
       </c>
       <c r="G10" s="53"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" s="11">
-        <v>2.6385908834798801</v>
+        <v>2.6587627546822699</v>
       </c>
       <c r="C11" s="11">
-        <v>0.471696508606186</v>
+        <v>0.468552072788116</v>
       </c>
       <c r="D11" s="11">
-        <v>51.036025588374102</v>
+        <v>51.029603104962803</v>
       </c>
       <c r="E11" s="11">
-        <v>5.5938317018216699</v>
+        <v>5.6744232052188499</v>
       </c>
       <c r="F11" s="69" t="s">
         <v>16</v>
       </c>
       <c r="G11" s="53"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="54" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="11">
-        <v>2.1247108825996301</v>
+        <v>2.0665791256694899</v>
       </c>
       <c r="C12" s="11">
-        <v>1.7763167781385401</v>
+        <v>1.7678469174003399</v>
       </c>
       <c r="D12" s="11">
-        <v>56.664038275812302</v>
+        <v>56.7473116383198</v>
       </c>
       <c r="E12" s="11">
-        <v>1.19613286816228</v>
+        <v>1.1689808123819001</v>
       </c>
       <c r="F12" s="62">
-        <v>0.23662596859941901</v>
+        <v>0.24729848658431</v>
       </c>
       <c r="G12" s="53"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="54" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="11">
-        <v>2.6895113611484698</v>
+        <v>2.5208764213502399</v>
       </c>
       <c r="C13" s="11">
-        <v>1.5985276393312899</v>
+        <v>1.5916890881333099</v>
       </c>
       <c r="D13" s="11">
-        <v>56.996121870834997</v>
+        <v>56.999155690105802</v>
       </c>
       <c r="E13" s="11">
-        <v>1.6824928734254301</v>
+        <v>1.58377439422334</v>
       </c>
       <c r="F13" s="62">
-        <v>9.7944519844202799E-2</v>
+        <v>0.118778312774835</v>
       </c>
       <c r="G13" s="53"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="54" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B14" s="11">
-        <v>-0.99701466622299395</v>
+        <v>-0.95784732924910498</v>
       </c>
       <c r="C14" s="11">
-        <v>0.61823987229120603</v>
+        <v>0.614173393116763</v>
       </c>
       <c r="D14" s="11">
-        <v>51.435380235414002</v>
+        <v>51.411269096953099</v>
       </c>
       <c r="E14" s="11">
-        <v>-1.6126663952100699</v>
+        <v>-1.5595715151193501</v>
       </c>
       <c r="F14" s="62">
-        <v>0.112936635710609</v>
+        <v>0.12499639205108801</v>
       </c>
       <c r="G14" s="53"/>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="57" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B15" s="20">
-        <v>-1.1514742262002999</v>
+        <v>-1.05724061082043</v>
       </c>
       <c r="C15" s="20">
-        <v>0.55508903286514999</v>
+        <v>0.55148457769854997</v>
       </c>
       <c r="D15" s="20">
-        <v>51.804378778902802</v>
+        <v>51.765396798592803</v>
       </c>
       <c r="E15" s="20">
-        <v>-2.0743955618377901</v>
-      </c>
-      <c r="F15" s="70">
-        <v>4.3028575472920501E-2</v>
+        <v>-1.91708100928678</v>
+      </c>
+      <c r="F15" s="63">
+        <v>6.0754506354321801E-2</v>
       </c>
       <c r="G15" s="58"/>
     </row>
@@ -3660,17 +3681,17 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.26953125" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="73" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="74"/>
       <c r="C1" s="74"/>
@@ -3679,9 +3700,9 @@
       <c r="F1" s="74"/>
       <c r="G1" s="74"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
@@ -3690,13 +3711,13 @@
       <c r="F2" s="50"/>
       <c r="G2" s="51"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="52"/>
       <c r="B3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>62</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>4</v>
@@ -3711,15 +3732,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" s="10">
-        <v>99.228999999999999</v>
+        <v>104.65</v>
       </c>
       <c r="C4" s="10">
-        <v>99.228999999999999</v>
+        <v>104.65</v>
       </c>
       <c r="D4" s="10">
         <v>1</v>
@@ -3728,21 +3749,21 @@
         <v>57</v>
       </c>
       <c r="F4" s="10">
-        <v>17.320399999999999</v>
+        <v>17</v>
       </c>
       <c r="G4" s="68" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="10">
-        <v>28.088000000000001</v>
+        <v>29.48</v>
       </c>
       <c r="C5" s="10">
-        <v>14.044</v>
+        <v>14.74</v>
       </c>
       <c r="D5" s="10">
         <v>2</v>
@@ -3751,21 +3772,21 @@
         <v>57</v>
       </c>
       <c r="F5" s="10">
-        <v>2.4512999999999998</v>
+        <v>2.39</v>
       </c>
       <c r="G5" s="67">
-        <v>9.5217300000000005E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" s="10">
-        <v>40.223999999999997</v>
+        <v>41.89</v>
       </c>
       <c r="C6" s="10">
-        <v>20.111999999999998</v>
+        <v>20.94</v>
       </c>
       <c r="D6" s="10">
         <v>2</v>
@@ -3774,13 +3795,13 @@
         <v>57</v>
       </c>
       <c r="F6" s="10">
-        <v>3.5106000000000002</v>
+        <v>3.4</v>
       </c>
       <c r="G6" s="68">
-        <v>3.64938E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="54"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -3789,9 +3810,9 @@
       <c r="F7" s="10"/>
       <c r="G7" s="53"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="55" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
@@ -3800,7 +3821,7 @@
       <c r="F8" s="59"/>
       <c r="G8" s="56"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="54"/>
       <c r="B9" s="29" t="s">
         <v>18</v>
@@ -3819,129 +3840,129 @@
       </c>
       <c r="G9" s="53"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="54" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="11">
-        <v>-23.36195361</v>
+        <v>-22.988770550080702</v>
       </c>
       <c r="C10" s="11">
-        <v>8.0427777230000004</v>
+        <v>8.3394034790433107</v>
       </c>
       <c r="D10" s="10">
-        <v>57.000003669999998</v>
+        <v>57</v>
       </c>
       <c r="E10" s="11">
-        <v>-2.9047120799999999</v>
+        <v>-2.7566444779714598</v>
       </c>
       <c r="F10" s="69">
-        <v>5.2232650000000004E-3</v>
+        <v>7.8304374593822796E-3</v>
       </c>
       <c r="G10" s="53"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" s="11">
-        <v>8.3165031860000003</v>
+        <v>8.3248917801398399</v>
       </c>
       <c r="C11" s="11">
-        <v>2.8669067909999999</v>
+        <v>2.97264120553643</v>
       </c>
       <c r="D11" s="10">
-        <v>57.000003669999998</v>
+        <v>57</v>
       </c>
       <c r="E11" s="11">
-        <v>2.9008627740000001</v>
+        <v>2.8005033922812599</v>
       </c>
       <c r="F11" s="69">
-        <v>5.2793689999999999E-3</v>
+        <v>6.9545520679667999E-3</v>
       </c>
       <c r="G11" s="53"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="54" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="11">
-        <v>11.71595411</v>
+        <v>10.853977231451401</v>
       </c>
       <c r="C12" s="11">
-        <v>8.8371710060000002</v>
+        <v>9.1630947877778404</v>
       </c>
       <c r="D12" s="10">
-        <v>57.000003669999998</v>
+        <v>57</v>
       </c>
       <c r="E12" s="11">
-        <v>1.3257584469999999</v>
+        <v>1.18453180752085</v>
       </c>
       <c r="F12" s="62">
-        <v>0.19020853099999999</v>
+        <v>0.24111832882845599</v>
       </c>
       <c r="G12" s="53"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="54" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="11">
-        <v>17.290429899999999</v>
+        <v>17.1483490289556</v>
       </c>
       <c r="C13" s="11">
-        <v>8.4780875370000004</v>
+        <v>8.7907679575763105</v>
       </c>
       <c r="D13" s="10">
-        <v>57.000003669999998</v>
+        <v>57</v>
       </c>
       <c r="E13" s="11">
-        <v>2.0394257339999999</v>
+        <v>1.95072252068448</v>
       </c>
       <c r="F13" s="69">
-        <v>4.6052975000000003E-2</v>
+        <v>5.6012504407177803E-2</v>
       </c>
       <c r="G13" s="53"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="54" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B14" s="11">
-        <v>-4.2764228099999997</v>
+        <v>-3.9945923421753</v>
       </c>
       <c r="C14" s="11">
-        <v>3.1555447879999998</v>
+        <v>3.27192446257884</v>
       </c>
       <c r="D14" s="10">
-        <v>57.000003669999998</v>
+        <v>57</v>
       </c>
       <c r="E14" s="11">
-        <v>-1.355209036</v>
+        <v>-1.22086936537247</v>
       </c>
       <c r="F14" s="62">
-        <v>0.18069733099999999</v>
+        <v>0.22716174662112101</v>
       </c>
       <c r="G14" s="53"/>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="57" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B15" s="20">
-        <v>-6.9823545149999999</v>
+        <v>-6.9202085275919298</v>
       </c>
       <c r="C15" s="20">
-        <v>3.0138652389999998</v>
+        <v>3.1250196292772201</v>
       </c>
       <c r="D15" s="19">
-        <v>57.000003669999998</v>
+        <v>57</v>
       </c>
       <c r="E15" s="20">
-        <v>-2.3167441019999999</v>
+        <v>-2.2144528190347699</v>
       </c>
       <c r="F15" s="70">
-        <v>2.4134165999999999E-2</v>
+        <v>3.0811593047039201E-2</v>
       </c>
       <c r="G15" s="58"/>
     </row>
@@ -3955,22 +3976,22 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.81640625" customWidth="1"/>
-    <col min="2" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="2" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="73" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="73"/>
       <c r="C1" s="73"/>
@@ -3979,9 +4000,9 @@
       <c r="F1" s="73"/>
       <c r="G1" s="73"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
@@ -3991,13 +4012,13 @@
       <c r="G2" s="51"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="52"/>
       <c r="B3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>62</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>4</v>
@@ -4013,241 +4034,251 @@
       </c>
       <c r="H3" s="37"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" s="10">
-        <v>398.07</v>
+        <v>404.01</v>
       </c>
       <c r="C4" s="10">
-        <v>398.07</v>
+        <v>404.01</v>
       </c>
       <c r="D4" s="10">
         <v>1</v>
       </c>
       <c r="E4" s="10">
-        <v>214.61</v>
+        <v>214.76</v>
       </c>
       <c r="F4" s="10">
-        <v>251.19300000000001</v>
+        <v>241.79</v>
       </c>
       <c r="G4" s="65" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="H4" s="37"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="10">
-        <v>31.41</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="C5" s="10">
-        <v>15.71</v>
+        <v>16.649999999999999</v>
       </c>
       <c r="D5" s="10">
         <v>2</v>
       </c>
       <c r="E5" s="10">
-        <v>243.37</v>
+        <v>243.56</v>
       </c>
       <c r="F5" s="10">
-        <v>9.9109999999999996</v>
+        <v>9.9700000000000006</v>
       </c>
       <c r="G5" s="65" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="H5" s="37"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" s="10">
-        <v>81.34</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="C6" s="10">
-        <v>40.67</v>
+        <v>39.950000000000003</v>
       </c>
       <c r="D6" s="10">
         <v>2</v>
       </c>
       <c r="E6" s="10">
-        <v>215.96</v>
+        <v>216.05</v>
       </c>
       <c r="F6" s="10">
-        <v>25.664999999999999</v>
+        <v>23.91</v>
       </c>
       <c r="G6" s="65" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="H6" s="37"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="60"/>
-      <c r="B8" s="28" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="54"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="37"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="60"/>
+      <c r="B9" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C9" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D9" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E9" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F9" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="61"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="54" t="s">
+      <c r="G9" s="61"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="30">
-        <v>-5.40735382</v>
-      </c>
-      <c r="C9" s="30">
-        <v>0.70216215100000001</v>
-      </c>
-      <c r="D9" s="30">
-        <v>163.87651030000001</v>
-      </c>
-      <c r="E9" s="30">
-        <v>-7.7010044110000004</v>
-      </c>
-      <c r="F9" s="64" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="53"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="54" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="11">
-        <v>2.7106336519999998</v>
-      </c>
-      <c r="C10" s="11">
-        <v>0.23875027300000001</v>
-      </c>
-      <c r="D10" s="11">
-        <v>214.3975915</v>
-      </c>
-      <c r="E10" s="11">
-        <v>11.3534264</v>
+      <c r="B10" s="30">
+        <v>-5.1265021910416904</v>
+      </c>
+      <c r="C10" s="30">
+        <v>0.71598084069326196</v>
+      </c>
+      <c r="D10" s="30">
+        <v>183.103295439752</v>
+      </c>
+      <c r="E10" s="30">
+        <v>-7.1601108572651997</v>
       </c>
       <c r="F10" s="64" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="G10" s="53"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="54" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B11" s="11">
-        <v>0.777339322</v>
+        <v>2.6848122716533198</v>
       </c>
       <c r="C11" s="11">
-        <v>0.85379192100000001</v>
+        <v>0.24514039399918799</v>
       </c>
       <c r="D11" s="11">
-        <v>243.5035235</v>
+        <v>214.459971232686</v>
       </c>
       <c r="E11" s="11">
-        <v>0.910455232</v>
-      </c>
-      <c r="F11" s="62">
-        <v>0.36348283599999998</v>
+        <v>10.952141455978101</v>
+      </c>
+      <c r="F11" s="64" t="s">
+        <v>71</v>
       </c>
       <c r="G11" s="53"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="11">
-        <v>3.1130718740000001</v>
+        <v>0.48294891366586301</v>
       </c>
       <c r="C12" s="11">
-        <v>0.81484029199999997</v>
+        <v>0.875514885138301</v>
       </c>
       <c r="D12" s="11">
-        <v>243.9567203</v>
+        <v>243.35432833207599</v>
       </c>
       <c r="E12" s="11">
-        <v>3.8204687509999999</v>
-      </c>
-      <c r="F12" s="64" t="s">
-        <v>81</v>
+        <v>0.55161702201050999</v>
+      </c>
+      <c r="F12" s="62">
+        <v>0.58199999999999996</v>
       </c>
       <c r="G12" s="53"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="54" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="B13" s="11">
-        <v>-1.111452173</v>
+        <v>3.0313122550844498</v>
       </c>
       <c r="C13" s="11">
-        <v>0.28908138900000002</v>
+        <v>0.83546727418728695</v>
       </c>
       <c r="D13" s="11">
-        <v>215.1346829</v>
+        <v>243.89827423923199</v>
       </c>
       <c r="E13" s="11">
-        <v>-3.8447724910000001</v>
+        <v>3.6282836548363901</v>
       </c>
       <c r="F13" s="64" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="G13" s="53"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="57" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="20">
-        <v>-1.9288279589999999</v>
-      </c>
-      <c r="C14" s="20">
-        <v>0.276341954</v>
-      </c>
-      <c r="D14" s="20">
-        <v>215.43466950000001</v>
-      </c>
-      <c r="E14" s="20">
-        <v>-6.9798593149999997</v>
-      </c>
-      <c r="F14" s="66" t="s">
-        <v>81</v>
-      </c>
-      <c r="G14" s="58"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="11">
+        <v>-1.03323561898946</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0.29681840768838003</v>
+      </c>
+      <c r="D14" s="11">
+        <v>215.19777215297501</v>
+      </c>
+      <c r="E14" s="11">
+        <v>-3.4810361898923001</v>
+      </c>
+      <c r="F14" s="64" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="53"/>
       <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="20">
+        <v>-1.89276356306045</v>
+      </c>
+      <c r="C15" s="20">
+        <v>0.28373807228954701</v>
+      </c>
+      <c r="D15" s="20">
+        <v>215.49707073196899</v>
+      </c>
+      <c r="E15" s="20">
+        <v>-6.6708127950095397</v>
+      </c>
+      <c r="F15" s="66" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="58"/>
+      <c r="H15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>